<commit_message>
for presentation in 240402
</commit_message>
<xml_diff>
--- a/data/中金量化测试数据.xlsx
+++ b/data/中金量化测试数据.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3590\Desktop\新需求\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\3590\Desktop\自动化项目工程文件\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D14A68C-EEAF-4809-A5B9-699C0B2FF3AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41D3C7B5-6CA2-409E-A7C4-7E296092B409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="36" yWindow="1248" windowWidth="17664" windowHeight="10632" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -560,9 +560,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -845,8 +844,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19:A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -872,7 +871,7 @@
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="1">
+      <c r="B3">
         <v>1</v>
       </c>
     </row>
@@ -880,7 +879,7 @@
       <c r="A4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1">
+      <c r="B4">
         <v>1</v>
       </c>
     </row>
@@ -888,7 +887,7 @@
       <c r="A5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="1">
+      <c r="B5">
         <v>1</v>
       </c>
     </row>
@@ -896,7 +895,7 @@
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="1">
+      <c r="B6">
         <v>1</v>
       </c>
     </row>
@@ -904,7 +903,7 @@
       <c r="A7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="1">
+      <c r="B7">
         <v>1</v>
       </c>
     </row>
@@ -912,7 +911,7 @@
       <c r="A8" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="1">
+      <c r="B8">
         <v>1</v>
       </c>
     </row>
@@ -920,7 +919,7 @@
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1">
+      <c r="B9">
         <v>1.002</v>
       </c>
     </row>
@@ -928,7 +927,7 @@
       <c r="A10" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="1">
+      <c r="B10">
         <v>1.0049999999999999</v>
       </c>
     </row>
@@ -936,7 +935,7 @@
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="1">
+      <c r="B11">
         <v>1.0049999999999999</v>
       </c>
     </row>
@@ -944,7 +943,7 @@
       <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="1">
+      <c r="B12">
         <v>1.0049999999999999</v>
       </c>
     </row>
@@ -952,7 +951,7 @@
       <c r="A13" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="1">
+      <c r="B13">
         <v>1.0069999999999999</v>
       </c>
     </row>
@@ -960,7 +959,7 @@
       <c r="A14" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="1">
+      <c r="B14">
         <v>1.0069999999999999</v>
       </c>
     </row>
@@ -968,7 +967,7 @@
       <c r="A15" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="1">
+      <c r="B15">
         <v>1.012</v>
       </c>
     </row>
@@ -976,7 +975,7 @@
       <c r="A16" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16">
         <v>1.0229999999999999</v>
       </c>
     </row>
@@ -984,7 +983,7 @@
       <c r="A17" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="1">
+      <c r="B17">
         <v>1.028</v>
       </c>
     </row>
@@ -992,7 +991,7 @@
       <c r="A18" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="1">
+      <c r="B18">
         <v>1.038</v>
       </c>
     </row>
@@ -1000,7 +999,7 @@
       <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="1">
+      <c r="B19">
         <v>1.0669999999999999</v>
       </c>
     </row>
@@ -1008,7 +1007,7 @@
       <c r="A20" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20">
         <v>1.0720000000000001</v>
       </c>
     </row>
@@ -1016,7 +1015,7 @@
       <c r="A21" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21">
         <v>1.077</v>
       </c>
     </row>
@@ -1024,7 +1023,7 @@
       <c r="A22" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="1">
+      <c r="B22">
         <v>1.1060000000000001</v>
       </c>
     </row>
@@ -1032,7 +1031,7 @@
       <c r="A23" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23">
         <v>1.121</v>
       </c>
     </row>
@@ -1040,7 +1039,7 @@
       <c r="A24" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="1">
+      <c r="B24">
         <v>1.119</v>
       </c>
     </row>
@@ -1048,7 +1047,7 @@
       <c r="A25" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="1">
+      <c r="B25">
         <v>1.135</v>
       </c>
     </row>
@@ -1056,7 +1055,7 @@
       <c r="A26" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="1">
+      <c r="B26">
         <v>1.129</v>
       </c>
     </row>
@@ -1064,7 +1063,7 @@
       <c r="A27" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="1">
+      <c r="B27">
         <v>1.1379999999999999</v>
       </c>
     </row>
@@ -1072,7 +1071,7 @@
       <c r="A28" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="1">
+      <c r="B28">
         <v>1.173</v>
       </c>
     </row>
@@ -1080,7 +1079,7 @@
       <c r="A29" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B29">
         <v>1.1775</v>
       </c>
     </row>
@@ -1088,7 +1087,7 @@
       <c r="A30" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="1">
+      <c r="B30">
         <v>1.2000999999999999</v>
       </c>
     </row>
@@ -1096,7 +1095,7 @@
       <c r="A31" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="1">
+      <c r="B31">
         <v>1.1934</v>
       </c>
     </row>
@@ -1104,7 +1103,7 @@
       <c r="A32" t="s">
         <v>31</v>
       </c>
-      <c r="B32" s="1">
+      <c r="B32">
         <v>1.2137</v>
       </c>
     </row>
@@ -1112,7 +1111,7 @@
       <c r="A33" t="s">
         <v>32</v>
       </c>
-      <c r="B33" s="1">
+      <c r="B33">
         <v>1.2317</v>
       </c>
     </row>
@@ -1120,7 +1119,7 @@
       <c r="A34" t="s">
         <v>33</v>
       </c>
-      <c r="B34" s="1">
+      <c r="B34">
         <v>1.2565999999999999</v>
       </c>
     </row>
@@ -1128,7 +1127,7 @@
       <c r="A35" t="s">
         <v>34</v>
       </c>
-      <c r="B35" s="1">
+      <c r="B35">
         <v>1.2475000000000001</v>
       </c>
     </row>
@@ -1136,7 +1135,7 @@
       <c r="A36" t="s">
         <v>35</v>
       </c>
-      <c r="B36" s="1">
+      <c r="B36">
         <v>1.2679</v>
       </c>
     </row>
@@ -1144,7 +1143,7 @@
       <c r="A37" t="s">
         <v>36</v>
       </c>
-      <c r="B37" s="1">
+      <c r="B37">
         <v>1.2735000000000001</v>
       </c>
     </row>
@@ -1152,7 +1151,7 @@
       <c r="A38" t="s">
         <v>37</v>
       </c>
-      <c r="B38" s="1">
+      <c r="B38">
         <v>1.2791999999999999</v>
       </c>
     </row>
@@ -1160,7 +1159,7 @@
       <c r="A39" t="s">
         <v>38</v>
       </c>
-      <c r="B39" s="1">
+      <c r="B39">
         <v>1.2984</v>
       </c>
     </row>
@@ -1168,7 +1167,7 @@
       <c r="A40" t="s">
         <v>39</v>
       </c>
-      <c r="B40" s="1">
+      <c r="B40">
         <v>1.3050999999999999</v>
       </c>
     </row>
@@ -1176,7 +1175,7 @@
       <c r="A41" t="s">
         <v>40</v>
       </c>
-      <c r="B41" s="1">
+      <c r="B41">
         <v>1.3174999999999999</v>
       </c>
     </row>
@@ -1184,7 +1183,7 @@
       <c r="A42" t="s">
         <v>41</v>
       </c>
-      <c r="B42" s="1">
+      <c r="B42">
         <v>1.3142</v>
       </c>
     </row>
@@ -1192,7 +1191,7 @@
       <c r="A43" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="1">
+      <c r="B43">
         <v>1.3355999999999999</v>
       </c>
     </row>
@@ -1200,7 +1199,7 @@
       <c r="A44" t="s">
         <v>43</v>
       </c>
-      <c r="B44" s="1">
+      <c r="B44">
         <v>1.3367</v>
       </c>
     </row>
@@ -1208,7 +1207,7 @@
       <c r="A45" t="s">
         <v>44</v>
       </c>
-      <c r="B45" s="1">
+      <c r="B45">
         <v>1.3604000000000001</v>
       </c>
     </row>
@@ -1216,7 +1215,7 @@
       <c r="A46" t="s">
         <v>45</v>
       </c>
-      <c r="B46" s="1">
+      <c r="B46">
         <v>1.3729</v>
       </c>
     </row>
@@ -1224,7 +1223,7 @@
       <c r="A47" t="s">
         <v>46</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B47">
         <v>1.3637999999999999</v>
       </c>
     </row>
@@ -1232,7 +1231,7 @@
       <c r="A48" t="s">
         <v>47</v>
       </c>
-      <c r="B48" s="1">
+      <c r="B48">
         <v>1.3808</v>
       </c>
     </row>
@@ -1240,7 +1239,7 @@
       <c r="A49" t="s">
         <v>48</v>
       </c>
-      <c r="B49" s="1">
+      <c r="B49">
         <v>1.3706</v>
       </c>
     </row>
@@ -1248,7 +1247,7 @@
       <c r="A50" t="s">
         <v>49</v>
       </c>
-      <c r="B50" s="1">
+      <c r="B50">
         <v>1.3875</v>
       </c>
     </row>
@@ -1256,7 +1255,7 @@
       <c r="A51" t="s">
         <v>50</v>
       </c>
-      <c r="B51" s="1">
+      <c r="B51">
         <v>1.4056</v>
       </c>
     </row>
@@ -1264,7 +1263,7 @@
       <c r="A52" t="s">
         <v>51</v>
       </c>
-      <c r="B52" s="1">
+      <c r="B52">
         <v>1.4159999999999999</v>
       </c>
     </row>
@@ -1272,7 +1271,7 @@
       <c r="A53" t="s">
         <v>52</v>
       </c>
-      <c r="B53" s="1">
+      <c r="B53">
         <v>1.4231</v>
       </c>
     </row>
@@ -1280,7 +1279,7 @@
       <c r="A54" t="s">
         <v>53</v>
       </c>
-      <c r="B54" s="1">
+      <c r="B54">
         <v>1.3822000000000001</v>
       </c>
     </row>
@@ -1288,7 +1287,7 @@
       <c r="A55" t="s">
         <v>54</v>
       </c>
-      <c r="B55" s="1">
+      <c r="B55">
         <v>1.4076</v>
       </c>
     </row>
@@ -1296,7 +1295,7 @@
       <c r="A56" t="s">
         <v>55</v>
       </c>
-      <c r="B56" s="1">
+      <c r="B56">
         <v>1.4146000000000001</v>
       </c>
     </row>
@@ -1304,7 +1303,7 @@
       <c r="A57" t="s">
         <v>56</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B57">
         <v>1.4668000000000001</v>
       </c>
     </row>
@@ -1312,7 +1311,7 @@
       <c r="A58" t="s">
         <v>57</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B58">
         <v>1.4879</v>
       </c>
     </row>
@@ -1320,7 +1319,7 @@
       <c r="A59" t="s">
         <v>58</v>
       </c>
-      <c r="B59" s="1">
+      <c r="B59">
         <v>1.5175000000000001</v>
       </c>
     </row>
@@ -1328,7 +1327,7 @@
       <c r="A60" t="s">
         <v>59</v>
       </c>
-      <c r="B60" s="1">
+      <c r="B60">
         <v>1.5287999999999999</v>
       </c>
     </row>
@@ -1336,7 +1335,7 @@
       <c r="A61" t="s">
         <v>60</v>
       </c>
-      <c r="B61" s="1">
+      <c r="B61">
         <v>1.5230999999999999</v>
       </c>
     </row>
@@ -1344,7 +1343,7 @@
       <c r="A62" t="s">
         <v>61</v>
       </c>
-      <c r="B62" s="1">
+      <c r="B62">
         <v>1.5611999999999999</v>
       </c>
     </row>
@@ -1352,7 +1351,7 @@
       <c r="A63" t="s">
         <v>62</v>
       </c>
-      <c r="B63" s="1">
+      <c r="B63">
         <v>1.5443</v>
       </c>
     </row>
@@ -1360,7 +1359,7 @@
       <c r="A64" t="s">
         <v>63</v>
       </c>
-      <c r="B64" s="1">
+      <c r="B64">
         <v>1.5427999999999999</v>
       </c>
     </row>
@@ -1368,7 +1367,7 @@
       <c r="A65" t="s">
         <v>64</v>
       </c>
-      <c r="B65" s="1">
+      <c r="B65">
         <v>1.5879000000000001</v>
       </c>
     </row>
@@ -1376,7 +1375,7 @@
       <c r="A66" t="s">
         <v>65</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B66">
         <v>1.5908</v>
       </c>
     </row>
@@ -1384,7 +1383,7 @@
       <c r="A67" t="s">
         <v>66</v>
       </c>
-      <c r="B67" s="1">
+      <c r="B67">
         <v>1.5908</v>
       </c>
     </row>
@@ -1392,7 +1391,7 @@
       <c r="A68" t="s">
         <v>67</v>
       </c>
-      <c r="B68" s="1">
+      <c r="B68">
         <v>1.6400999999999999</v>
       </c>
     </row>
@@ -1400,7 +1399,7 @@
       <c r="A69" t="s">
         <v>68</v>
       </c>
-      <c r="B69" s="1">
+      <c r="B69">
         <v>1.6456999999999999</v>
       </c>
     </row>
@@ -1408,7 +1407,7 @@
       <c r="A70" t="s">
         <v>69</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B70">
         <v>1.6626000000000001</v>
       </c>
     </row>
@@ -1416,7 +1415,7 @@
       <c r="A71" t="s">
         <v>70</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B71">
         <v>1.6626000000000001</v>
       </c>
     </row>
@@ -1424,7 +1423,7 @@
       <c r="A72" t="s">
         <v>71</v>
       </c>
-      <c r="B72" s="1">
+      <c r="B72">
         <v>1.6639999999999999</v>
       </c>
     </row>
@@ -1432,7 +1431,7 @@
       <c r="A73" t="s">
         <v>72</v>
       </c>
-      <c r="B73" s="1">
+      <c r="B73">
         <v>1.7049000000000001</v>
       </c>
     </row>
@@ -1440,7 +1439,7 @@
       <c r="A74" t="s">
         <v>73</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B74">
         <v>1.7415</v>
       </c>
     </row>
@@ -1448,7 +1447,7 @@
       <c r="A75" t="s">
         <v>74</v>
       </c>
-      <c r="B75" s="1">
+      <c r="B75">
         <v>1.7091000000000001</v>
       </c>
     </row>
@@ -1456,7 +1455,7 @@
       <c r="A76" t="s">
         <v>75</v>
       </c>
-      <c r="B76" s="1">
+      <c r="B76">
         <v>1.7359</v>
       </c>
     </row>
@@ -1464,7 +1463,7 @@
       <c r="A77" t="s">
         <v>76</v>
       </c>
-      <c r="B77" s="1">
+      <c r="B77">
         <v>1.7401</v>
       </c>
     </row>
@@ -1472,7 +1471,7 @@
       <c r="A78" t="s">
         <v>77</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B78">
         <v>1.7765</v>
       </c>
     </row>
@@ -1480,7 +1479,7 @@
       <c r="A79" t="s">
         <v>78</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B79">
         <v>1.7467999999999999</v>
       </c>
     </row>
@@ -1488,7 +1487,7 @@
       <c r="A80" t="s">
         <v>79</v>
       </c>
-      <c r="B80" s="1">
+      <c r="B80">
         <v>1.7451000000000001</v>
       </c>
     </row>
@@ -1496,7 +1495,7 @@
       <c r="A81" t="s">
         <v>80</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B81">
         <v>1.7695000000000001</v>
       </c>
     </row>
@@ -1504,7 +1503,7 @@
       <c r="A82" t="s">
         <v>81</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B82">
         <v>1.766</v>
       </c>
     </row>
@@ -1512,7 +1511,7 @@
       <c r="A83" t="s">
         <v>82</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B83">
         <v>1.7887999999999999</v>
       </c>
     </row>
@@ -1520,7 +1519,7 @@
       <c r="A84" t="s">
         <v>83</v>
       </c>
-      <c r="B84" s="1">
+      <c r="B84">
         <v>1.7853000000000001</v>
       </c>
     </row>
@@ -1528,7 +1527,7 @@
       <c r="A85" t="s">
         <v>84</v>
       </c>
-      <c r="B85" s="1">
+      <c r="B85">
         <v>1.7992999999999999</v>
       </c>
     </row>
@@ -1536,7 +1535,7 @@
       <c r="A86" t="s">
         <v>85</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B86">
         <v>1.7958000000000001</v>
       </c>
     </row>
@@ -1544,7 +1543,7 @@
       <c r="A87" t="s">
         <v>86</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B87">
         <v>1.8045</v>
       </c>
     </row>
@@ -1552,7 +1551,7 @@
       <c r="A88" t="s">
         <v>87</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B88">
         <v>1.8063</v>
       </c>
     </row>
@@ -1560,7 +1559,7 @@
       <c r="A89" t="s">
         <v>88</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B89">
         <v>1.7975000000000001</v>
       </c>
     </row>
@@ -1568,7 +1567,7 @@
       <c r="A90" t="s">
         <v>89</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B90">
         <v>1.7975000000000001</v>
       </c>
     </row>
@@ -1576,7 +1575,7 @@
       <c r="A91" t="s">
         <v>90</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B91">
         <v>1.7975000000000001</v>
       </c>
     </row>
@@ -1584,7 +1583,7 @@
       <c r="A92" t="s">
         <v>91</v>
       </c>
-      <c r="B92" s="1">
+      <c r="B92">
         <v>1.7958000000000001</v>
       </c>
     </row>
@@ -1592,7 +1591,7 @@
       <c r="A93" t="s">
         <v>92</v>
       </c>
-      <c r="B93" s="1">
+      <c r="B93">
         <v>1.7869999999999999</v>
       </c>
     </row>
@@ -1600,7 +1599,7 @@
       <c r="A94" t="s">
         <v>93</v>
       </c>
-      <c r="B94" s="1">
+      <c r="B94">
         <v>1.7887999999999999</v>
       </c>
     </row>
@@ -1608,7 +1607,7 @@
       <c r="A95" t="s">
         <v>94</v>
       </c>
-      <c r="B95" s="1">
+      <c r="B95">
         <v>1.7887999999999999</v>
       </c>
     </row>
@@ -1616,7 +1615,7 @@
       <c r="A96" t="s">
         <v>95</v>
       </c>
-      <c r="B96" s="1">
+      <c r="B96">
         <v>1.7905</v>
       </c>
     </row>
@@ -1624,7 +1623,7 @@
       <c r="A97" t="s">
         <v>96</v>
       </c>
-      <c r="B97" s="1">
+      <c r="B97">
         <v>1.794</v>
       </c>
     </row>
@@ -1632,7 +1631,7 @@
       <c r="A98" t="s">
         <v>97</v>
       </c>
-      <c r="B98" s="1">
+      <c r="B98">
         <v>1.7975000000000001</v>
       </c>
     </row>
@@ -1640,7 +1639,7 @@
       <c r="A99" t="s">
         <v>98</v>
       </c>
-      <c r="B99" s="1">
+      <c r="B99">
         <v>1.7905</v>
       </c>
     </row>
@@ -1648,7 +1647,7 @@
       <c r="A100" t="s">
         <v>99</v>
       </c>
-      <c r="B100" s="1">
+      <c r="B100">
         <v>1.7923</v>
       </c>
     </row>
@@ -1656,7 +1655,7 @@
       <c r="A101" t="s">
         <v>100</v>
       </c>
-      <c r="B101" s="1">
+      <c r="B101">
         <v>1.7869999999999999</v>
       </c>
     </row>
@@ -1664,7 +1663,7 @@
       <c r="A102" t="s">
         <v>101</v>
       </c>
-      <c r="B102" s="1">
+      <c r="B102">
         <v>1.8009999999999999</v>
       </c>
     </row>
@@ -1672,7 +1671,7 @@
       <c r="A103" t="s">
         <v>102</v>
       </c>
-      <c r="B103" s="1">
+      <c r="B103">
         <v>1.7678</v>
       </c>
     </row>
@@ -1680,7 +1679,7 @@
       <c r="A104" t="s">
         <v>103</v>
       </c>
-      <c r="B104" s="1">
+      <c r="B104">
         <v>1.7625</v>
       </c>
     </row>
@@ -1688,7 +1687,7 @@
       <c r="A105" t="s">
         <v>104</v>
       </c>
-      <c r="B105" s="1">
+      <c r="B105">
         <v>1.7729999999999999</v>
       </c>
     </row>
@@ -1696,7 +1695,7 @@
       <c r="A106" t="s">
         <v>105</v>
       </c>
-      <c r="B106" s="1">
+      <c r="B106">
         <v>1.7869999999999999</v>
       </c>
     </row>
@@ -1704,7 +1703,7 @@
       <c r="A107" t="s">
         <v>106</v>
       </c>
-      <c r="B107" s="1">
+      <c r="B107">
         <v>1.766</v>
       </c>
     </row>
@@ -1712,7 +1711,7 @@
       <c r="A108" t="s">
         <v>107</v>
       </c>
-      <c r="B108" s="1">
+      <c r="B108">
         <v>1.7521</v>
       </c>
     </row>
@@ -1720,7 +1719,7 @@
       <c r="A109" t="s">
         <v>108</v>
       </c>
-      <c r="B109" s="1">
+      <c r="B109">
         <v>1.7416</v>
       </c>
     </row>
@@ -1728,7 +1727,7 @@
       <c r="A110" t="s">
         <v>109</v>
       </c>
-      <c r="B110" s="1">
+      <c r="B110">
         <v>1.7765</v>
       </c>
     </row>
@@ -1736,7 +1735,7 @@
       <c r="A111" t="s">
         <v>110</v>
       </c>
-      <c r="B111" s="1">
+      <c r="B111">
         <v>1.7783</v>
       </c>
     </row>
@@ -1744,7 +1743,7 @@
       <c r="A112" t="s">
         <v>111</v>
       </c>
-      <c r="B112" s="1">
+      <c r="B112">
         <v>1.7765</v>
       </c>
     </row>
@@ -1752,7 +1751,7 @@
       <c r="A113" t="s">
         <v>112</v>
       </c>
-      <c r="B113" s="1">
+      <c r="B113">
         <v>1.7992999999999999</v>
       </c>
     </row>
@@ -1760,7 +1759,7 @@
       <c r="A114" t="s">
         <v>113</v>
       </c>
-      <c r="B114" s="1">
+      <c r="B114">
         <v>1.8080000000000001</v>
       </c>
     </row>
@@ -1768,7 +1767,7 @@
       <c r="A115" t="s">
         <v>114</v>
       </c>
-      <c r="B115" s="1">
+      <c r="B115">
         <v>1.8098000000000001</v>
       </c>
     </row>
@@ -1776,7 +1775,7 @@
       <c r="A116" t="s">
         <v>115</v>
       </c>
-      <c r="B116" s="1">
+      <c r="B116">
         <v>1.8185</v>
       </c>
     </row>
@@ -1784,7 +1783,7 @@
       <c r="A117" t="s">
         <v>116</v>
       </c>
-      <c r="B117" s="1">
+      <c r="B117">
         <v>1.8307</v>
       </c>
     </row>
@@ -1792,7 +1791,7 @@
       <c r="A118" t="s">
         <v>117</v>
       </c>
-      <c r="B118" s="1">
+      <c r="B118">
         <v>1.8325</v>
       </c>
     </row>
@@ -1800,7 +1799,7 @@
       <c r="A119" t="s">
         <v>118</v>
       </c>
-      <c r="B119" s="1">
+      <c r="B119">
         <v>1.843</v>
       </c>
     </row>
@@ -1808,7 +1807,7 @@
       <c r="A120" t="s">
         <v>119</v>
       </c>
-      <c r="B120" s="1">
+      <c r="B120">
         <v>1.8482000000000001</v>
       </c>
     </row>
@@ -1816,7 +1815,7 @@
       <c r="A121" t="s">
         <v>120</v>
       </c>
-      <c r="B121" s="1">
+      <c r="B121">
         <v>1.8534999999999999</v>
       </c>
     </row>
@@ -1824,7 +1823,7 @@
       <c r="A122" t="s">
         <v>121</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B122">
         <v>1.8674999999999999</v>
       </c>
     </row>
@@ -1832,7 +1831,7 @@
       <c r="A123" t="s">
         <v>122</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B123">
         <v>1.8815</v>
       </c>
     </row>
@@ -1840,7 +1839,7 @@
       <c r="A124" t="s">
         <v>123</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B124">
         <v>1.8954</v>
       </c>
     </row>
@@ -1848,7 +1847,7 @@
       <c r="A125" t="s">
         <v>124</v>
       </c>
-      <c r="B125" s="1">
+      <c r="B125">
         <v>1.9007000000000001</v>
       </c>
     </row>
@@ -1856,7 +1855,7 @@
       <c r="A126" t="s">
         <v>125</v>
       </c>
-      <c r="B126" s="1">
+      <c r="B126">
         <v>1.9234</v>
       </c>
     </row>
@@ -1864,7 +1863,7 @@
       <c r="A127" t="s">
         <v>126</v>
       </c>
-      <c r="B127" s="1">
+      <c r="B127">
         <v>1.9217</v>
       </c>
     </row>
@@ -1872,7 +1871,7 @@
       <c r="A128" t="s">
         <v>127</v>
       </c>
-      <c r="B128" s="1">
+      <c r="B128">
         <v>1.9217</v>
       </c>
     </row>
@@ -1880,7 +1879,7 @@
       <c r="A129" t="s">
         <v>128</v>
       </c>
-      <c r="B129" s="1">
+      <c r="B129">
         <v>1.9392</v>
       </c>
     </row>
@@ -1888,7 +1887,7 @@
       <c r="A130" t="s">
         <v>129</v>
       </c>
-      <c r="B130" s="1">
+      <c r="B130">
         <v>1.9409000000000001</v>
       </c>
     </row>
@@ -1896,7 +1895,7 @@
       <c r="A131" t="s">
         <v>130</v>
       </c>
-      <c r="B131" s="1">
+      <c r="B131">
         <v>1.9654</v>
       </c>
     </row>
@@ -1904,7 +1903,7 @@
       <c r="A132" t="s">
         <v>131</v>
       </c>
-      <c r="B132" s="1">
+      <c r="B132">
         <v>1.9951000000000001</v>
       </c>
     </row>
@@ -1912,7 +1911,7 @@
       <c r="A133" t="s">
         <v>132</v>
       </c>
-      <c r="B133" s="1">
+      <c r="B133">
         <v>2.0230999999999999</v>
       </c>
     </row>
@@ -1920,7 +1919,7 @@
       <c r="A134" t="s">
         <v>133</v>
       </c>
-      <c r="B134" s="1">
+      <c r="B134">
         <v>2.0230999999999999</v>
       </c>
     </row>
@@ -1928,7 +1927,7 @@
       <c r="A135" t="s">
         <v>134</v>
       </c>
-      <c r="B135" s="1">
+      <c r="B135">
         <v>2.0440999999999998</v>
       </c>
     </row>
@@ -1936,7 +1935,7 @@
       <c r="A136" t="s">
         <v>135</v>
       </c>
-      <c r="B136" s="1">
+      <c r="B136">
         <v>2.0493000000000001</v>
       </c>
     </row>
@@ -1944,7 +1943,7 @@
       <c r="A137" t="s">
         <v>136</v>
       </c>
-      <c r="B137" s="1">
+      <c r="B137">
         <v>2.0842999999999998</v>
       </c>
     </row>
@@ -1952,7 +1951,7 @@
       <c r="A138" t="s">
         <v>137</v>
       </c>
-      <c r="B138" s="1">
+      <c r="B138">
         <v>2.0859999999999999</v>
       </c>
     </row>
@@ -1960,7 +1959,7 @@
       <c r="A139" t="s">
         <v>138</v>
       </c>
-      <c r="B139" s="1">
+      <c r="B139">
         <v>2.1053000000000002</v>
       </c>
     </row>
@@ -1968,7 +1967,7 @@
       <c r="A140" t="s">
         <v>139</v>
       </c>
-      <c r="B140" s="1">
+      <c r="B140">
         <v>2.1</v>
       </c>
     </row>
@@ -1976,7 +1975,7 @@
       <c r="A141" t="s">
         <v>140</v>
       </c>
-      <c r="B141" s="1">
+      <c r="B141">
         <v>2.0983000000000001</v>
       </c>
     </row>
@@ -1984,7 +1983,7 @@
       <c r="A142" t="s">
         <v>141</v>
       </c>
-      <c r="B142" s="1">
+      <c r="B142">
         <v>2.1332</v>
       </c>
     </row>
@@ -1992,7 +1991,7 @@
       <c r="A143" t="s">
         <v>142</v>
       </c>
-      <c r="B143" s="1">
+      <c r="B143">
         <v>2.1402000000000001</v>
       </c>
     </row>
@@ -2000,7 +1999,7 @@
       <c r="A144" t="s">
         <v>143</v>
       </c>
-      <c r="B144" s="1">
+      <c r="B144">
         <v>2.1261999999999999</v>
       </c>
     </row>
@@ -2008,7 +2007,7 @@
       <c r="A145" t="s">
         <v>144</v>
       </c>
-      <c r="B145" s="1">
+      <c r="B145">
         <v>2.1366999999999998</v>
       </c>
     </row>
@@ -2016,7 +2015,7 @@
       <c r="A146" t="s">
         <v>145</v>
       </c>
-      <c r="B146" s="1">
+      <c r="B146">
         <v>2.1297000000000001</v>
       </c>
     </row>
@@ -2024,7 +2023,7 @@
       <c r="A147" t="s">
         <v>146</v>
       </c>
-      <c r="B147" s="1">
+      <c r="B147">
         <v>2.1541999999999999</v>
       </c>
     </row>
@@ -2032,7 +2031,7 @@
       <c r="A148" t="s">
         <v>147</v>
       </c>
-      <c r="B148" s="1">
+      <c r="B148">
         <v>2.1595</v>
       </c>
     </row>
@@ -2040,7 +2039,7 @@
       <c r="A149" t="s">
         <v>148</v>
       </c>
-      <c r="B149" s="1">
+      <c r="B149">
         <v>2.1577000000000002</v>
       </c>
     </row>
@@ -2048,7 +2047,7 @@
       <c r="A150" t="s">
         <v>149</v>
       </c>
-      <c r="B150" s="1">
+      <c r="B150">
         <v>2.1821999999999999</v>
       </c>
     </row>
@@ -2056,7 +2055,7 @@
       <c r="A151" t="s">
         <v>150</v>
       </c>
-      <c r="B151" s="1">
+      <c r="B151">
         <v>2.1787000000000001</v>
       </c>
     </row>
@@ -2064,7 +2063,7 @@
       <c r="A152" t="s">
         <v>151</v>
       </c>
-      <c r="B152" s="1">
+      <c r="B152">
         <v>2.1821999999999999</v>
       </c>
     </row>
@@ -2072,7 +2071,7 @@
       <c r="A153" t="s">
         <v>152</v>
       </c>
-      <c r="B153" s="1">
+      <c r="B153">
         <v>2.1909000000000001</v>
       </c>
     </row>
@@ -2080,7 +2079,7 @@
       <c r="A154" t="s">
         <v>153</v>
       </c>
-      <c r="B154" s="1">
+      <c r="B154">
         <v>2.1943999999999999</v>
       </c>
     </row>
@@ -2088,7 +2087,7 @@
       <c r="A155" t="s">
         <v>154</v>
       </c>
-      <c r="B155" s="1">
+      <c r="B155">
         <v>2.1979000000000002</v>
       </c>
     </row>
@@ -2096,7 +2095,7 @@
       <c r="A156" t="s">
         <v>155</v>
       </c>
-      <c r="B156" s="1">
+      <c r="B156">
         <v>2.1943999999999999</v>
       </c>
     </row>
@@ -2104,7 +2103,7 @@
       <c r="A157" t="s">
         <v>156</v>
       </c>
-      <c r="B157" s="1">
+      <c r="B157">
         <v>2.1926999999999999</v>
       </c>
     </row>
@@ -2112,7 +2111,7 @@
       <c r="A158" t="s">
         <v>157</v>
       </c>
-      <c r="B158" s="1">
+      <c r="B158">
         <v>2.1979000000000002</v>
       </c>
     </row>
@@ -2120,7 +2119,7 @@
       <c r="A159" t="s">
         <v>158</v>
       </c>
-      <c r="B159" s="1">
+      <c r="B159">
         <v>2.1979000000000002</v>
       </c>
     </row>
@@ -2128,7 +2127,7 @@
       <c r="A160" t="s">
         <v>159</v>
       </c>
-      <c r="B160" s="1">
+      <c r="B160">
         <v>2.2101999999999999</v>
       </c>
     </row>
@@ -2136,7 +2135,7 @@
       <c r="A161" t="s">
         <v>160</v>
       </c>
-      <c r="B161" s="1">
+      <c r="B161">
         <v>2.2172000000000001</v>
       </c>
     </row>
@@ -2144,7 +2143,7 @@
       <c r="A162" t="s">
         <v>161</v>
       </c>
-      <c r="B162" s="1">
+      <c r="B162">
         <v>2.2311999999999999</v>
       </c>
     </row>
@@ -2152,7 +2151,7 @@
       <c r="A163" t="s">
         <v>162</v>
       </c>
-      <c r="B163" s="1">
+      <c r="B163">
         <v>2.2259000000000002</v>
       </c>
     </row>
@@ -2160,7 +2159,7 @@
       <c r="A164" t="s">
         <v>163</v>
       </c>
-      <c r="B164" s="1">
+      <c r="B164">
         <v>2.2242000000000002</v>
       </c>
     </row>

</xml_diff>